<commit_message>
update june 30 est
</commit_message>
<xml_diff>
--- a/june 30 est.xlsx
+++ b/june 30 est.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karlp\Documents\cashflow\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E05708E9-8CFC-4189-8F01-1B84E04933B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2030BC39-BCB2-4F64-934A-37362180511A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5625" yWindow="555" windowWidth="16875" windowHeight="9195" xr2:uid="{A08A0D8E-2D16-4C1D-A633-5B8F83758C04}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Estimating 6/30 returns with known information</t>
   </si>
@@ -50,9 +50,6 @@
     <t>times 22%</t>
   </si>
   <si>
-    <t>Real estate (guestimate)</t>
-  </si>
-  <si>
     <t>times 17%</t>
   </si>
   <si>
@@ -62,15 +59,9 @@
     <t>add Q4 estimates</t>
   </si>
   <si>
-    <t>Bonds (actual through april 15)</t>
-  </si>
-  <si>
     <t>times 10%</t>
   </si>
   <si>
-    <t>Stocks (actual through april 15)</t>
-  </si>
-  <si>
     <t>times 40%</t>
   </si>
   <si>
@@ -83,10 +74,13 @@
     <t xml:space="preserve">Required stock market gain rest of quarter to get to zero </t>
   </si>
   <si>
-    <t>SPX on 4/15</t>
-  </si>
-  <si>
-    <t>SPX needs to be on 6/30</t>
+    <t>Real estate (estimate)</t>
+  </si>
+  <si>
+    <t>Bonds (actual through april 29)</t>
+  </si>
+  <si>
+    <t>Stocks (actual through april 29)</t>
   </si>
 </sst>
 </file>
@@ -461,9 +455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4B394A-5CEC-4AC3-87B0-45141A24D757}">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -487,10 +479,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3">
-        <v>-4.2</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="C6" s="3">
         <v>-3.2</v>
@@ -502,7 +494,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -512,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="3">
-        <v>-2.9</v>
+        <v>-2.2000000000000002</v>
       </c>
       <c r="C9" s="3">
         <v>-12.4</v>
@@ -524,7 +516,7 @@
       </c>
       <c r="B10" s="3">
         <f>B9*0.22</f>
-        <v>-0.63800000000000001</v>
+        <v>-0.48400000000000004</v>
       </c>
       <c r="C10" s="3">
         <f>C9*0.22</f>
@@ -537,26 +529,26 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="C12" s="3">
-        <v>-5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="3">
         <f>B12*0.17</f>
-        <v>-0.51</v>
+        <v>-0.34</v>
       </c>
       <c r="C13" s="3">
         <f>C12*0.17</f>
-        <v>-0.85000000000000009</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -565,28 +557,26 @@
     </row>
     <row r="15" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B15" s="3">
-        <f>100*(117/115-1)</f>
-        <v>1.7391304347825987</v>
+        <v>2.4</v>
       </c>
       <c r="C15" s="3">
-        <f>B15</f>
-        <v>1.7391304347825987</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" s="3">
         <f>B15*0.1</f>
-        <v>0.17391304347825987</v>
+        <v>0.24</v>
       </c>
       <c r="C16" s="3">
         <f>C15*0.1</f>
-        <v>0.17391304347825987</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.45">
@@ -595,28 +585,26 @@
     </row>
     <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B18" s="3">
-        <f>100*(-1+65.6/62.5)</f>
-        <v>4.9599999999999866</v>
+        <v>17</v>
       </c>
       <c r="C18" s="3">
-        <f>B18</f>
-        <v>4.9599999999999866</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B19" s="3">
         <f>B18*0.4</f>
-        <v>1.9839999999999947</v>
+        <v>6.8000000000000007</v>
       </c>
       <c r="C19" s="3">
         <f>C18*0.4</f>
-        <v>1.9839999999999947</v>
+        <v>6.8000000000000007</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -625,7 +613,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B21" s="3">
         <v>-10</v>
@@ -636,7 +624,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B22">
         <f>B21*0.1</f>
@@ -649,53 +637,33 @@
     </row>
     <row r="24" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B24" s="2">
         <f>B22+B19+B16+B13+B10+B6</f>
-        <v>-4.1900869565217453</v>
+        <v>1.1160000000000014</v>
       </c>
       <c r="C24" s="2">
         <f>C22+C19+C16+C13+C10+C6</f>
-        <v>-6.6200869565217459</v>
+        <v>-0.71799999999999953</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B26" s="2">
         <f>-B24*2.5</f>
-        <v>10.475217391304364</v>
+        <v>-2.7900000000000036</v>
       </c>
       <c r="C26" s="2">
         <f>-C24*2.5</f>
-        <v>16.550217391304365</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28">
-        <v>2783</v>
-      </c>
-      <c r="C28">
-        <v>2783</v>
+        <v>1.7949999999999988</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>17</v>
-      </c>
-      <c r="B29" s="2">
-        <f>B28*(1+B26*0.01)</f>
-        <v>3074.5253000000007</v>
-      </c>
-      <c r="C29" s="2">
-        <f>C28*(1+C26*0.01)</f>
-        <v>3243.5925500000003</v>
-      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>